<commit_message>
Changed image used for test
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/justsch_student_ubc_ca/Documents/Documents/Work/sbits_spline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44683898-C56A-47B4-9974-DB5A26D3CBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{44683898-C56A-47B4-9974-DB5A26D3CBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{957F9A91-8A26-4D2F-8FA8-410D604E9670}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CC67C65B-E3A4-4136-9BE8-948B3E0092DA}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="46">
   <si>
     <t>Num Runs</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>FS</t>
+  </si>
+  <si>
+    <t>Commit:</t>
+  </si>
+  <si>
+    <t>https://github.com/ubco-db/sbits_spline/commit/f9bfa4bf96a991a978191489e6f7c122c010d971</t>
   </si>
 </sst>
 </file>
@@ -545,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9A9ED0-9CEF-4E06-A760-3A7A6D319452}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,6 +647,14 @@
         <v>43</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
@@ -650,9 +664,10 @@
     <hyperlink ref="B11" location="'Fixed-Justin-May-19'!A1" display="JF" xr:uid="{38C547CA-9B6D-42A1-8CC5-A4B7D678895B}"/>
     <hyperlink ref="C10" location="'Var-Seth-May-19'!A1" display="SV" xr:uid="{9DDAEEF4-1AED-4938-B7A9-9FEC33DB1419}"/>
     <hyperlink ref="C11" location="'Fixed-Seth-May-19'!A1" display="FS" xr:uid="{0AF2E073-BE57-481B-BF78-41AEEDEC01CA}"/>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{AF5EBE6B-6B33-4702-AF5D-9E4EE97F75E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>